<commit_message>
VR monthly 04/23 Virtual Reality
</commit_message>
<xml_diff>
--- a/Monthly/03-02 VR/fig3_data_soltani_and_morice_2023.xlsx
+++ b/Monthly/03-02 VR/fig3_data_soltani_and_morice_2023.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsp5/Documents/GitHub/open-source/Monthly/03-02 VR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C695100-F5BA-9440-BF6E-350A021BA9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02475E2C-7552-7548-BD30-4F883D7EE510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{D1FFD21E-AF7B-1E44-B72F-02AF7931C56E}"/>
+    <workbookView xWindow="2600" yWindow="2260" windowWidth="27640" windowHeight="16940" xr2:uid="{D1FFD21E-AF7B-1E44-B72F-02AF7931C56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,18 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
   <si>
-    <t>angle</t>
-  </si>
-  <si>
-    <t>velocity</t>
-  </si>
-  <si>
-    <t>angle_sd</t>
-  </si>
-  <si>
-    <t>velocity_sd</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -69,6 +57,18 @@
   </si>
   <si>
     <t>distance_m</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>depth_sd</t>
+  </si>
+  <si>
+    <t>side_sd</t>
   </si>
 </sst>
 </file>
@@ -423,316 +423,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408EF6B4-2830-CF43-8D97-1E095D7AE012}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4.7391362683438096</v>
+      </c>
+      <c r="B2">
+        <v>5.0095765199161404</v>
+      </c>
+      <c r="C2">
+        <v>-4.5333333333333198E-2</v>
+      </c>
+      <c r="D2">
+        <v>-0.14133333333333301</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5.2249999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4.7515136268343801</v>
+      </c>
+      <c r="B3">
+        <v>4.9967966457023003</v>
+      </c>
+      <c r="C3">
+        <v>1.8666666666666599E-2</v>
+      </c>
+      <c r="D3">
+        <v>7.7333333333333198E-2</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.2249999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4.3300461215932904</v>
+      </c>
+      <c r="B4">
+        <v>4.6445283018867896</v>
+      </c>
+      <c r="C4">
+        <v>4.5333333333333399E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.3333333333333393E-2</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5.2249999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4.6759077568134098</v>
+      </c>
+      <c r="B5">
+        <v>4.8457190775681296</v>
+      </c>
+      <c r="C5">
+        <v>6.1333333333333198E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.12533333333333299</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5.2249999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4.1855765199161397</v>
+      </c>
+      <c r="B6">
+        <v>4.3931069182389901</v>
+      </c>
+      <c r="C6">
+        <v>-1.33333333333334E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.9333333333333201E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>60.672010688042697</v>
-      </c>
-      <c r="B2" s="1">
-        <v>6.8308617234468896</v>
-      </c>
-      <c r="C2" s="1">
-        <v>61.523862539894601</v>
-      </c>
-      <c r="D2" s="1">
-        <v>6.9014028056112204</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3.2225000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>61.787946262896099</v>
-      </c>
-      <c r="B3" s="1">
-        <v>7.03927855711422</v>
-      </c>
-      <c r="C3" s="1">
-        <v>62.565724040673899</v>
-      </c>
-      <c r="D3" s="1">
-        <v>7.1162324649298503</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1">
-        <v>3.2225000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>64.528909671194199</v>
-      </c>
-      <c r="B4" s="1">
-        <v>7.0488977955911798</v>
-      </c>
-      <c r="C4" s="1">
-        <v>65.9733541156386</v>
-      </c>
-      <c r="D4" s="1">
-        <v>7.1418837675350604</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3.2225000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>63.048096192384698</v>
-      </c>
-      <c r="B5" s="1">
-        <v>7.0777555110220396</v>
-      </c>
-      <c r="C5" s="1">
-        <v>64.492540636829204</v>
-      </c>
-      <c r="D5" s="1">
-        <v>7.2893787575150197</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3.2225000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>58.309953239812899</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7.18997995991983</v>
-      </c>
-      <c r="C6" s="1">
-        <v>58.3119572478289</v>
-      </c>
-      <c r="D6" s="1">
-        <v>7.27655310621242</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G6" s="1">
         <v>4.2249999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>57.6459585838343</v>
-      </c>
-      <c r="B7" s="1">
-        <v>7.3054108216432798</v>
-      </c>
-      <c r="C7" s="1">
-        <v>59.349662287538003</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7.3599198396793497</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
+      <c r="A7">
+        <v>4.2546247379454902</v>
+      </c>
+      <c r="B7">
+        <v>4.4118406708595304</v>
+      </c>
+      <c r="C7">
+        <v>2.9333333333333201E-2</v>
+      </c>
+      <c r="D7">
+        <v>9.3333333333333393E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <v>4.2249999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>63.688784977362097</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7.5555110220440804</v>
-      </c>
-      <c r="C8" s="1">
-        <v>65.244340532917604</v>
-      </c>
-      <c r="D8" s="1">
-        <v>7.7254509018036002</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
+      <c r="A8">
+        <v>4.0092243186582799</v>
+      </c>
+      <c r="B8">
+        <v>4.1790356394129899</v>
+      </c>
+      <c r="C8">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.14133333333333301</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
       </c>
       <c r="G8" s="1">
         <v>4.2249999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>62.757960365174696</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7.3438877755511003</v>
-      </c>
-      <c r="C9" s="1">
-        <v>63.202479032138299</v>
-      </c>
-      <c r="D9" s="1">
-        <v>7.4400801603206403</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>9</v>
+      <c r="A9">
+        <v>4.2861719077568097</v>
+      </c>
+      <c r="B9">
+        <v>4.4245534591194904</v>
+      </c>
+      <c r="C9">
+        <v>-2.6666666666665898E-3</v>
+      </c>
+      <c r="D9">
+        <v>4.5333333333333399E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
       </c>
       <c r="G9" s="1">
         <v>4.2249999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>58.7250055666889</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7.5202404809619203</v>
-      </c>
-      <c r="C10" s="1">
-        <v>59.243524085207397</v>
-      </c>
-      <c r="D10" s="1">
-        <v>7.6100200400801503</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
+      <c r="A10">
+        <v>3.5691740041928699</v>
+      </c>
+      <c r="B10">
+        <v>3.76410901467505</v>
+      </c>
+      <c r="C10">
+        <v>2.6666666666668101E-3</v>
+      </c>
+      <c r="D10">
+        <v>-7.7333333333333407E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
       </c>
       <c r="G10" s="1">
-        <v>5.2249999999999996</v>
+        <v>3.2250000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>58.172567356936</v>
-      </c>
-      <c r="B11" s="1">
-        <v>7.6549098196392702</v>
-      </c>
-      <c r="C11" s="1">
-        <v>59.691011652935501</v>
-      </c>
-      <c r="D11" s="1">
-        <v>7.7318637274548996</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>8</v>
+      <c r="A11">
+        <v>3.5502222222222199</v>
+      </c>
+      <c r="B11">
+        <v>3.7766373165618399</v>
+      </c>
+      <c r="C11">
+        <v>2.9333333333333201E-2</v>
+      </c>
+      <c r="D11">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
       </c>
       <c r="G11" s="1">
-        <v>5.2249999999999996</v>
+        <v>3.2250000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>63.216878200846097</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7.9691382765530996</v>
-      </c>
-      <c r="C12" s="1">
-        <v>64.327915089438093</v>
-      </c>
-      <c r="D12" s="1">
-        <v>8.09739478957915</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
+      <c r="A12">
+        <v>3.7136603773584902</v>
+      </c>
+      <c r="B12">
+        <v>3.9274968553459102</v>
+      </c>
+      <c r="C12">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
       </c>
       <c r="G12" s="1">
-        <v>5.2249999999999996</v>
+        <v>3.2250000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>60.649818154828097</v>
-      </c>
-      <c r="B13" s="1">
-        <v>7.4721442885771499</v>
-      </c>
-      <c r="C13" s="1">
-        <v>62.316484821494797</v>
-      </c>
-      <c r="D13" s="1">
-        <v>7.5266533066132197</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
+      <c r="A13">
+        <v>3.7138784067085902</v>
+      </c>
+      <c r="B13">
+        <v>3.8585324947589101</v>
+      </c>
+      <c r="C13">
+        <v>-1.33333333333334E-2</v>
+      </c>
+      <c r="D13">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
       </c>
       <c r="G13" s="1">
-        <v>5.2249999999999996</v>
-      </c>
+        <v>3.2250000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>